<commit_message>
Style add sheet title
</commit_message>
<xml_diff>
--- a/webscrapping/model.xlsx
+++ b/webscrapping/model.xlsx
@@ -14,11 +14,17 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <b/>
     </font>
   </fonts>
   <fills count="2">
@@ -40,8 +46,9 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -53,107 +60,107 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetData>
     <row r="1" spans="1:21">
-      <c r="A1" s="0" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>ID</t>
         </is>
       </c>
-      <c r="B1" s="0" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>Title</t>
         </is>
       </c>
-      <c r="C1" s="0" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Type</t>
         </is>
       </c>
-      <c r="D1" s="0" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Author 1</t>
         </is>
       </c>
-      <c r="E1" s="0" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Author 1 Institution</t>
         </is>
       </c>
-      <c r="F1" s="0" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Author 2</t>
         </is>
       </c>
-      <c r="G1" s="0" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Author 2 Institution</t>
         </is>
       </c>
-      <c r="H1" s="0" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Author 3</t>
         </is>
       </c>
-      <c r="I1" s="0" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Author 3 Institution</t>
         </is>
       </c>
-      <c r="J1" s="0" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Author 4</t>
         </is>
       </c>
-      <c r="K1" s="0" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Author 4 Institution</t>
         </is>
       </c>
-      <c r="L1" s="0" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>Author 5</t>
         </is>
       </c>
-      <c r="M1" s="0" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>Author 5 Institution</t>
         </is>
       </c>
-      <c r="N1" s="0" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>Author 6</t>
         </is>
       </c>
-      <c r="O1" s="0" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>Author 6 Institution</t>
         </is>
       </c>
-      <c r="P1" s="0" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>Author 7</t>
         </is>
       </c>
-      <c r="Q1" s="0" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>Author 7 Institution</t>
         </is>
       </c>
-      <c r="R1" s="0" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>Author 8</t>
         </is>
       </c>
-      <c r="S1" s="0" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>Author 8 Institution</t>
         </is>
       </c>
-      <c r="T1" s="0" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>Author 9</t>
         </is>
       </c>
-      <c r="U1" s="0" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>Author 9 Institution</t>
         </is>

</xml_diff>